<commit_message>
changed logic to pass excel sheet in run.py
</commit_message>
<xml_diff>
--- a/unit_test_cases/add.xlsx
+++ b/unit_test_cases/add.xlsx
@@ -91,13 +91,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -108,6 +114,12 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -483,118 +495,181 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="12.96" customWidth="1" style="4" min="1" max="1"/>
-    <col width="14.88" customWidth="1" style="4" min="3" max="4"/>
-    <col width="14.49" customWidth="1" style="4" min="5" max="5"/>
+    <col width="16.53" customWidth="1" style="6" min="1" max="1"/>
+    <col width="14.88" customWidth="1" style="6" min="3" max="4"/>
+    <col width="14.49" customWidth="1" style="6" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="5">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="12.8" customHeight="1" s="7">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>$INC_FILE</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>example/add.hpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="7">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>$FUNC_FILE</t>
+        </is>
+      </c>
+      <c r="B2" s="8" t="inlineStr">
+        <is>
+          <t>example/add.cpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="7">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>$INC_PATH_GCC</t>
+        </is>
+      </c>
+      <c r="B3" s="9" t="n"/>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="7">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>$FLAGS_GCC</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>-pthread</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="7">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>$FUNC_NAME</t>
+        </is>
+      </c>
+      <c r="B5" s="8" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="7">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>Test Case NO</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Param 1</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>Param 2</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D6" s="6" t="inlineStr">
         <is>
           <t>Expected Result</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>Result Obtained</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="5">
-      <c r="A2" s="4" t="n">
+    <row r="7" ht="12.8" customHeight="1" s="7">
+      <c r="A7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B7" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C7" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D7" s="6" t="n">
         <v>3.5</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E7" s="6" t="n">
         <v>3.5</v>
       </c>
-      <c r="F2" s="6" t="inlineStr">
+      <c r="F7" s="10" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="5">
-      <c r="A3" s="4" t="n">
+    <row r="8" ht="12.8" customHeight="1" s="7">
+      <c r="A8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B8" s="6" t="n">
         <v>3.1</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C8" s="6" t="n">
         <v>3.1</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D8" s="6" t="n">
         <v>6.2</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E8" s="6" t="n">
         <v>6.199999809265137</v>
       </c>
-      <c r="F3" s="7" t="inlineStr">
+      <c r="F8" s="11" t="inlineStr">
         <is>
           <t>FAIL</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="1" s="5">
-      <c r="A4" s="4" t="n">
+    <row r="9" ht="12.8" customHeight="1" s="7">
+      <c r="A9" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B9" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C9" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D9" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E9" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="F4" s="6" t="inlineStr">
+      <c r="F9" s="10" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+  </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>